<commit_message>
results of more verification work
</commit_message>
<xml_diff>
--- a/kiev_not_found_working.xlsx
+++ b/kiev_not_found_working.xlsx
@@ -233,7 +233,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,8 +263,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,6 +286,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -306,12 +318,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -325,8 +338,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,13 +649,20 @@
   <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" hidden="1" customWidth="1"/>
+    <col min="6" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" customWidth="1"/>
     <col min="17" max="17" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="41.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -826,65 +851,65 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>28</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="8">
         <v>208</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="2" t="s">
+      <c r="E4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="8">
         <v>42</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="S4" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="T4" s="8" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>